<commit_message>
# Remove any '_y' suffixed columns if their original column exists
</commit_message>
<xml_diff>
--- a/merged.xlsx
+++ b/merged.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD6"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -714,30 +714,25 @@
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Location txt</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>Location txt</t>
+          <t>EO provider</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>EO provider</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 10</t>
         </is>
@@ -912,26 +907,21 @@
           <t>5yz7fafspka5h0acz4hus5yz7rti6yb9</t>
         </is>
       </c>
-      <c r="AY2" s="2" t="inlineStr">
-        <is>
-          <t>Cal</t>
+      <c r="AY2" s="5" t="inlineStr">
+        <is>
+          <t>256-242-9976</t>
         </is>
       </c>
       <c r="AZ2" s="5" t="inlineStr">
         <is>
-          <t>256-242-9976</t>
-        </is>
-      </c>
-      <c r="BA2" s="5" t="inlineStr">
-        <is>
           <t>Hamilton</t>
         </is>
       </c>
-      <c r="BB2" s="5" t="inlineStr"/>
-      <c r="BC2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="5" t="inlineStr">
+      <c r="BA2" s="5" t="inlineStr"/>
+      <c r="BB2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="5" t="inlineStr">
         <is>
           <t>5yz7fafspka5h0acz4hus5yz7rti6yb9</t>
         </is>
@@ -1144,30 +1134,25 @@
           <t>ycgg7xjd5pqwo0nsllvycgg7xvxpf6k5</t>
         </is>
       </c>
-      <c r="AY3" s="2" t="inlineStr">
-        <is>
-          <t>Bob</t>
+      <c r="AY3" s="5" t="inlineStr">
+        <is>
+          <t>(719) 259- 9854</t>
         </is>
       </c>
       <c r="AZ3" s="5" t="inlineStr">
         <is>
-          <t>(719) 259- 9854</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="BA3" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="BB3" s="5" t="inlineStr">
-        <is>
           <t>rth</t>
         </is>
       </c>
-      <c r="BC3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD3" s="5" t="inlineStr">
+      <c r="BB3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="5" t="inlineStr">
         <is>
           <t>ycgg7xjd5pqwo0nsllvycgg7xvxpf6k5</t>
         </is>
@@ -1382,30 +1367,25 @@
           <t>mjr7u5nz6qic0e64vmjr7u5ycdf6akj6</t>
         </is>
       </c>
-      <c r="AY4" s="2" t="inlineStr">
-        <is>
-          <t>Stu</t>
+      <c r="AY4" s="5" t="inlineStr">
+        <is>
+          <t>(382)-719-2456</t>
         </is>
       </c>
       <c r="AZ4" s="5" t="inlineStr">
         <is>
-          <t>(382)-719-2456</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="BA4" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="BB4" s="5" t="inlineStr">
-        <is>
           <t>Toronto</t>
         </is>
       </c>
-      <c r="BC4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD4" s="5" t="inlineStr">
+      <c r="BB4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC4" s="5" t="inlineStr">
         <is>
           <t>mjr7u5nz6qic0e64vmjr7u5ycdf6akj6</t>
         </is>
@@ -1600,28 +1580,23 @@
         </is>
       </c>
       <c r="AX5" s="4" t="inlineStr"/>
-      <c r="AY5" s="2" t="inlineStr">
-        <is>
-          <t>Uncle</t>
-        </is>
-      </c>
-      <c r="AZ5" s="5" t="n">
+      <c r="AY5" s="5" t="n">
         <v>9993457586</v>
       </c>
+      <c r="AZ5" s="5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BA5" s="5" t="inlineStr">
         <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="BB5" s="5" t="inlineStr">
-        <is>
           <t>Oakville</t>
         </is>
       </c>
-      <c r="BC5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD5" s="5" t="inlineStr"/>
+      <c r="BB5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC5" s="5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -1804,30 +1779,25 @@
           <t>igbyr90ypthglwfyigbyhtvnrce8gswq</t>
         </is>
       </c>
-      <c r="AY6" s="2" t="inlineStr">
-        <is>
-          <t>Renée</t>
+      <c r="AY6" s="5" t="inlineStr">
+        <is>
+          <t>956-717-9023</t>
         </is>
       </c>
       <c r="AZ6" s="5" t="inlineStr">
         <is>
-          <t>956-717-9023</t>
+          <t>Hamilton</t>
         </is>
       </c>
       <c r="BA6" s="5" t="inlineStr">
         <is>
-          <t>Hamilton</t>
-        </is>
-      </c>
-      <c r="BB6" s="5" t="inlineStr">
-        <is>
           <t>Val D'Or</t>
         </is>
       </c>
-      <c r="BC6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="5" t="inlineStr">
+      <c r="BB6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="5" t="inlineStr">
         <is>
           <t>igbyr90ypthglwfyigbyhtvnrce8gswq</t>
         </is>

</xml_diff>